<commit_message>
Manual Testing Notes on 30th Oct
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\007 LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F132AE43-3CD9-429D-BA6D-E89DA9F98AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C926A-8848-41A4-8051-67673E80D2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42B6BE39-C700-4B85-A7B5-78554C539B19}"/>
   </bookViews>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0DE554-DD68-492A-B356-D1795EFDE9BC}">
   <dimension ref="A2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
     <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Sql notes and queries
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\007 LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C926A-8848-41A4-8051-67673E80D2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67ED46B-78E8-4D66-898B-D185476FBA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42B6BE39-C700-4B85-A7B5-78554C539B19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -179,6 +179,13 @@
   <si>
     <t>username textbox should accept text 
 entered and display the same</t>
+  </si>
+  <si>
+    <t>Click login button</t>
+  </si>
+  <si>
+    <t>Page shoulsd be navigated to
+"Search Hotel Page"</t>
   </si>
 </sst>
 </file>
@@ -275,13 +282,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -599,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0DE554-DD68-492A-B356-D1795EFDE9BC}">
   <dimension ref="A2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +619,7 @@
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
@@ -626,13 +633,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
@@ -644,13 +651,13 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
@@ -662,13 +669,13 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
@@ -680,13 +687,13 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
@@ -698,479 +705,483 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="63" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="84" x14ac:dyDescent="0.4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="84" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4" t="s">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="42" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
+      <c r="F12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="5"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="5"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>